<commit_message>
Format code, remove typo
</commit_message>
<xml_diff>
--- a/short.xlsx
+++ b/short.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://solisservices-my.sharepoint.com/personal/t_shahedi_uu_nl/Documents/Documents/ADS Task force/final version database/Shiny-ADS-AI-Courses/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\4216318\Desktop\shiny\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{F89C2AC3-E126-4694-AFFC-B7E8E5F4C12E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{05D833DB-4217-4219-BE23-46B358CD2463}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18DC9060-62A8-47E1-BA75-2396A65504C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -164,9 +164,6 @@
     <t>Exploratory Data Analysis</t>
   </si>
   <si>
-    <t>MplusÂ </t>
-  </si>
-  <si>
     <t>Statistics</t>
   </si>
   <si>
@@ -186,6 +183,9 @@
   </si>
   <si>
     <t>Relational databases</t>
+  </si>
+  <si>
+    <t>Mplus</t>
   </si>
 </sst>
 </file>
@@ -196,7 +196,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -505,17 +505,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="48.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.8984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -523,7 +523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -531,7 +531,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -539,7 +539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -547,7 +547,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -555,7 +555,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -563,7 +563,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -571,15 +571,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B8" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -587,7 +587,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -595,7 +595,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -603,7 +603,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -611,7 +611,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -619,7 +619,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -627,7 +627,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -635,7 +635,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -643,7 +643,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -651,7 +651,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -659,7 +659,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>11</v>
       </c>
@@ -667,7 +667,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -675,7 +675,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>13</v>
       </c>
@@ -683,7 +683,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>32</v>
       </c>
@@ -691,7 +691,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>33</v>
       </c>
@@ -699,7 +699,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>34</v>
       </c>
@@ -707,7 +707,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>35</v>
       </c>
@@ -715,7 +715,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>36</v>
       </c>
@@ -723,7 +723,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>37</v>
       </c>
@@ -731,7 +731,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>38</v>
       </c>
@@ -739,7 +739,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>39</v>
       </c>
@@ -747,7 +747,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>40</v>
       </c>
@@ -755,7 +755,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>14</v>
       </c>
@@ -763,7 +763,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>15</v>
       </c>
@@ -771,7 +771,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>16</v>
       </c>
@@ -779,7 +779,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>41</v>
       </c>
@@ -787,7 +787,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>22</v>
       </c>
@@ -795,15 +795,15 @@
         <v>22</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="B36" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>23</v>
       </c>
@@ -811,7 +811,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>24</v>
       </c>
@@ -819,7 +819,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>17</v>
       </c>
@@ -827,15 +827,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B40" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>18</v>
       </c>
@@ -843,7 +843,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>19</v>
       </c>
@@ -851,7 +851,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>20</v>
       </c>
@@ -859,7 +859,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>21</v>
       </c>
@@ -867,44 +867,44 @@
         <v>21</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
+        <v>43</v>
+      </c>
+      <c r="B45" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
         <v>44</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
         <v>45</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B47" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
         <v>46</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B48" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
         <v>47</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>48</v>
-      </c>
-      <c r="B49" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>